<commit_message>
Added code to add Queue Item for every test script listed in the Execution file.
</commit_message>
<xml_diff>
--- a/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Dispatcher/Data/Config.xlsx
+++ b/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Dispatcher/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandra.veizu\Documents\Reframework_update_UiPath_Services\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\srcCode\UiPath_TestAutomation_GenericAsset\TestAutomation_GenericAsset\TestAutomation_GenericAsset_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB87279-7458-4D58-83F7-8E2A5713A403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -90,19 +90,7 @@
     <t>Framework</t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>OrchestratorQueueName</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -122,6 +110,21 @@
   </si>
   <si>
     <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>Generic Asset</t>
+  </si>
+  <si>
+    <t>OrchestratorFolderPath</t>
+  </si>
+  <si>
+    <t>ExecutionQueue</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>FolderLocation_ExecutionFile</t>
   </si>
 </sst>
 </file>
@@ -497,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -547,28 +550,33 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="30">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1561,6 +1569,7 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1572,7 +1581,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -1624,7 +1635,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1648,7 +1659,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1670,7 +1681,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1681,7 +1692,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1692,7 +1703,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2675,15 +2686,16 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2702,7 +2714,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2730,7 +2742,17 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3728,9 +3750,9 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated name of the Asset "FolderLocation_ExecutionFiles"
</commit_message>
<xml_diff>
--- a/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Dispatcher/Data/Config.xlsx
+++ b/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Dispatcher/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\srcCode\UiPath_TestAutomation_GenericAsset\TestAutomation_GenericAsset\TestAutomation_GenericAsset_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB87279-7458-4D58-83F7-8E2A5713A403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2102B473-628D-41B9-AD5F-588A8909349C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -124,7 +124,7 @@
     <t>OrchestratorQueueName</t>
   </si>
   <si>
-    <t>FolderLocation_ExecutionFile</t>
+    <t>FolderLocation_ExecutionFiles</t>
   </si>
 </sst>
 </file>
@@ -2695,7 +2695,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
May 19, 2022 09:43 PM
</commit_message>
<xml_diff>
--- a/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Dispatcher/Data/Config.xlsx
+++ b/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Dispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\srcCode\UiPath_TestAutomation_GenericAsset\TestAutomation_GenericAsset\TestAutomation_GenericAsset_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2102B473-628D-41B9-AD5F-588A8909349C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50B17A7-AB76-47CF-9921-92E41444897A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13215" yWindow="3735" windowWidth="15750" windowHeight="10440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -125,6 +125,15 @@
   </si>
   <si>
     <t>FolderLocation_ExecutionFiles</t>
+  </si>
+  <si>
+    <t>FolderLocation_LogFiles</t>
+  </si>
+  <si>
+    <t>FolderLocation_Screenshots</t>
+  </si>
+  <si>
+    <t>FolderLocation_UserInterface</t>
   </si>
 </sst>
 </file>
@@ -2695,7 +2704,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2753,9 +2762,39 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
May 20, 2022 8:35 PM
</commit_message>
<xml_diff>
--- a/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Dispatcher/Data/Config.xlsx
+++ b/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Dispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\srcCode\UiPath_TestAutomation_GenericAsset\TestAutomation_GenericAsset\TestAutomation_GenericAsset_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50B17A7-AB76-47CF-9921-92E41444897A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CEAEEE-7DE2-4DA6-959A-BD7A3F7DCB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13215" yWindow="3735" windowWidth="15750" windowHeight="10440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>FolderLocation_UserInterface</t>
+  </si>
+  <si>
+    <t>ExecutionFile_SheetName</t>
+  </si>
+  <si>
+    <t>Delay_Short</t>
   </si>
 </sst>
 </file>
@@ -2704,7 +2710,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2795,8 +2801,28 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
October 10, 2022 04:28PM
</commit_message>
<xml_diff>
--- a/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Dispatcher/Data/Config.xlsx
+++ b/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Dispatcher/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\srcCode\UiPath_TestAutomation_GenericAsset\TestAutomation_GenericAsset\TestAutomation_GenericAsset_Dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath_TestAutomation_GenericAsset\TestAutomation_GenericAsset\TestAutomation_GenericAsset_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CEAEEE-7DE2-4DA6-959A-BD7A3F7DCB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C192CE5-B820-4BE2-9C08-C3F591F7E97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -112,9 +112,6 @@
     <t>OrchestratorAssetFolder</t>
   </si>
   <si>
-    <t>Generic Asset</t>
-  </si>
-  <si>
     <t>OrchestratorFolderPath</t>
   </si>
   <si>
@@ -140,6 +137,9 @@
   </si>
   <si>
     <t>Delay_Short</t>
+  </si>
+  <si>
+    <t>Downstream/International Products/IFL Automation</t>
   </si>
 </sst>
 </file>
@@ -521,12 +521,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -565,23 +565,23 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1600,12 +1600,12 @@
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1642,7 +1642,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2709,16 +2709,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2759,68 +2759,68 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
         <v>38</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>